<commit_message>
Finished initial alignment to Phenopackets v1.
</commit_message>
<xml_diff>
--- a/Biosample.xlsx
+++ b/Biosample.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$57</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="339">
   <si>
     <t>Path</t>
   </si>
@@ -150,7 +150,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Role[classCode=SPEC]</t>
@@ -165,7 +165,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -197,6 +197,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
     <t>Specimen.implicitRules</t>
   </si>
   <si>
@@ -319,6 +323,10 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
     <t>individualAgeAtCollection</t>
   </si>
   <si>
@@ -333,8 +341,67 @@
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+    <t>histologicalDiagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/biosample-histological-diagnosis}
+</t>
+  </si>
+  <si>
+    <t>The pathologist’s diagnosis.</t>
+  </si>
+  <si>
+    <t>tumorProgression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/biosample-tumor-progression}
+</t>
+  </si>
+  <si>
+    <t>This field can be used to indicate if a specimen is from the primary tumor, a metastasis or a recurrence.</t>
+  </si>
+  <si>
+    <t>tumorGrade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/biosample-tumor-grade}
+</t>
+  </si>
+  <si>
+    <t>List of terms representing the tumor grade.</t>
+  </si>
+  <si>
+    <t>diagnosticMarkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/biosample-diagnostic-markers}
+</t>
+  </si>
+  <si>
+    <t>Clinically relevant bio markers.</t>
+  </si>
+  <si>
+    <t>htsFiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/htsfiles}
+</t>
+  </si>
+  <si>
+    <t>List of high-throughput sequencing files generated as part of a genomic test.</t>
+  </si>
+  <si>
+    <t>variants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ga4gh.org/fhir/phenopackets/StructureDefinition/variants}
+</t>
+  </si>
+  <si>
+    <t>This is a field for genetic variants and can be used for listing either candidate variants or diagnosed causative variants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a field for genetic variants and can be used for listing either candidate variants or diagnosed causative variants. </t>
   </si>
   <si>
     <t>isControlSample</t>
@@ -425,7 +492,7 @@
     <t>Codes providing the status/availability of a specimen.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/specimen-status|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/specimen-status|4.0.1</t>
   </si>
   <si>
     <t>status</t>
@@ -572,10 +639,6 @@
     <t>Details concerning the specimen collection.</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
-  </si>
-  <si>
     <t>.participation[typeCode=SBJ].act[classCode=SPECCOLLECT, moodCode=EVN]</t>
   </si>
   <si>
@@ -583,10 +646,6 @@
   </si>
   <si>
     <t>Specimen.collection.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
   </si>
   <si>
     <t>Unique id for inter-element referencing</t>
@@ -1162,7 +1221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL51"/>
+  <dimension ref="A1:AL57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1635,7 +1694,7 @@
         <v>39</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>39</v>
@@ -1649,7 +1708,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1672,16 +1731,16 @@
         <v>48</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1731,7 +1790,7 @@
         <v>39</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>40</v>
@@ -1743,7 +1802,7 @@
         <v>39</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>39</v>
@@ -1757,7 +1816,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1780,16 +1839,16 @@
         <v>39</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1815,13 +1874,13 @@
         <v>39</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>39</v>
@@ -1839,7 +1898,7 @@
         <v>39</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>40</v>
@@ -1851,7 +1910,7 @@
         <v>39</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>39</v>
@@ -1865,11 +1924,11 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1888,16 +1947,16 @@
         <v>39</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1947,7 +2006,7 @@
         <v>39</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>40</v>
@@ -1959,10 +2018,10 @@
         <v>39</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>39</v>
@@ -1973,11 +2032,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1996,16 +2055,16 @@
         <v>39</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2055,7 +2114,7 @@
         <v>39</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>40</v>
@@ -2070,7 +2129,7 @@
         <v>39</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>39</v>
@@ -2081,7 +2140,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2104,13 +2163,13 @@
         <v>39</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2149,17 +2208,17 @@
         <v>39</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>40</v>
@@ -2171,7 +2230,7 @@
         <v>39</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>39</v>
@@ -2185,16 +2244,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s" s="2">
         <v>40</v>
@@ -2212,13 +2271,13 @@
         <v>39</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -2269,7 +2328,7 @@
         <v>39</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>40</v>
@@ -2278,10 +2337,10 @@
         <v>41</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>39</v>
@@ -2295,16 +2354,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s" s="2">
         <v>40</v>
@@ -2322,13 +2381,13 @@
         <v>39</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2379,7 +2438,7 @@
         <v>39</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -2388,10 +2447,10 @@
         <v>41</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>39</v>
@@ -2403,45 +2462,45 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" hidden="true">
+    <row r="12">
       <c r="A12" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>106</v>
+      </c>
       <c r="C12" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>39</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L12" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="M12" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N12" t="s" s="2">
-        <v>110</v>
-      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>39</v>
       </c>
@@ -2489,7 +2548,7 @@
         <v>39</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2498,13 +2557,13 @@
         <v>41</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>39</v>
@@ -2515,18 +2574,22 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>109</v>
+      </c>
       <c r="C13" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" t="s" s="2">
+        <v>109</v>
+      </c>
       <c r="E13" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>48</v>
@@ -2535,16 +2598,16 @@
         <v>39</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2595,7 +2658,7 @@
         <v>39</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2604,30 +2667,34 @@
         <v>41</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>118</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="C14" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="E14" t="s" s="2">
         <v>40</v>
       </c>
@@ -2635,22 +2702,22 @@
         <v>47</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s" s="2">
         <v>113</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2701,66 +2768,68 @@
         <v>39</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="E15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="AL14" t="s" s="2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" hidden="true">
-      <c r="A15" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H15" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="I15" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J15" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="K15" t="s" s="2">
-        <v>125</v>
-      </c>
       <c r="L15" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>127</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>39</v>
@@ -2785,13 +2854,13 @@
         <v>39</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>129</v>
+        <v>39</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>130</v>
+        <v>39</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>39</v>
@@ -2809,44 +2878,48 @@
         <v>39</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>133</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>118</v>
+      </c>
       <c r="C16" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" t="s" s="2">
+        <v>118</v>
+      </c>
       <c r="E16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>48</v>
@@ -2855,20 +2928,18 @@
         <v>39</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>138</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>39</v>
@@ -2893,13 +2964,13 @@
         <v>39</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>39</v>
@@ -2917,39 +2988,43 @@
         <v>39</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>144</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>122</v>
+      </c>
       <c r="C17" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" t="s" s="2">
+        <v>122</v>
+      </c>
       <c r="E17" t="s" s="2">
         <v>40</v>
       </c>
@@ -2963,21 +3038,19 @@
         <v>39</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" t="s" s="2">
-        <v>149</v>
-      </c>
+      <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>39</v>
       </c>
@@ -3025,25 +3098,25 @@
         <v>39</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>39</v>
@@ -3051,39 +3124,43 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="M18" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N18" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O18" t="s" s="2">
         <v>39</v>
       </c>
@@ -3131,33 +3208,33 @@
         <v>39</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>157</v>
+        <v>39</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>158</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3171,26 +3248,24 @@
         <v>41</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>163</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>39</v>
@@ -3239,7 +3314,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3251,21 +3326,21 @@
         <v>39</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>39</v>
+        <v>137</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3276,7 +3351,7 @@
         <v>40</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>39</v>
@@ -3285,20 +3360,18 @@
         <v>39</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>169</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>39</v>
@@ -3347,33 +3420,33 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>172</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3390,21 +3463,23 @@
         <v>39</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="M21" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>147</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>39</v>
@@ -3429,13 +3504,13 @@
         <v>39</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>39</v>
@@ -3453,7 +3528,7 @@
         <v>39</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3465,21 +3540,21 @@
         <v>39</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>177</v>
+        <v>59</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>179</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3493,24 +3568,26 @@
         <v>47</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>158</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>39</v>
@@ -3535,13 +3612,13 @@
         <v>39</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>39</v>
@@ -3559,7 +3636,7 @@
         <v>39</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3571,55 +3648,55 @@
         <v>39</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>39</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>91</v>
+        <v>166</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>168</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" t="s" s="2">
+        <v>169</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>39</v>
       </c>
@@ -3667,25 +3744,25 @@
         <v>39</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>39</v>
+        <v>171</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>39</v>
@@ -3693,43 +3770,39 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>191</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>39</v>
       </c>
@@ -3777,33 +3850,33 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>39</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3814,7 +3887,7 @@
         <v>40</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>39</v>
@@ -3823,18 +3896,20 @@
         <v>39</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>183</v>
+      </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>39</v>
@@ -3883,33 +3958,33 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>200</v>
+        <v>39</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>201</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3920,7 +3995,7 @@
         <v>40</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>39</v>
@@ -3929,18 +4004,20 @@
         <v>39</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>189</v>
+      </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>39</v>
@@ -3989,33 +4066,33 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4035,16 +4112,16 @@
         <v>39</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4095,7 +4172,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -4107,21 +4184,21 @@
         <v>39</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>39</v>
+        <v>197</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>207</v>
+        <v>39</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4144,13 +4221,13 @@
         <v>39</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>214</v>
+        <v>49</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4201,7 +4278,7 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4216,29 +4293,29 @@
         <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>218</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>39</v>
@@ -4250,15 +4327,17 @@
         <v>39</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M29" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>39</v>
@@ -4283,13 +4362,13 @@
         <v>39</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>222</v>
+        <v>39</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>223</v>
+        <v>39</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>39</v>
@@ -4307,67 +4386,69 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>225</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>39</v>
       </c>
@@ -4391,13 +4472,13 @@
         <v>39</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>230</v>
+        <v>39</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>231</v>
+        <v>39</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>39</v>
@@ -4415,33 +4496,33 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>232</v>
+        <v>90</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>233</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4464,20 +4545,16 @@
         <v>48</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>239</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>39</v>
       </c>
@@ -4501,13 +4578,13 @@
         <v>39</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>241</v>
+        <v>39</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>242</v>
+        <v>39</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>39</v>
@@ -4525,7 +4602,7 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4537,21 +4614,21 @@
         <v>39</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>39</v>
+        <v>217</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>243</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4562,7 +4639,7 @@
         <v>40</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>39</v>
@@ -4571,16 +4648,16 @@
         <v>39</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4631,33 +4708,33 @@
         <v>39</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>177</v>
+        <v>59</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>39</v>
+        <v>225</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>39</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4677,16 +4754,16 @@
         <v>39</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4737,7 +4814,7 @@
         <v>39</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -4749,13 +4826,13 @@
         <v>39</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>185</v>
+        <v>39</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>39</v>
+        <v>225</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>39</v>
@@ -4763,18 +4840,18 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>39</v>
@@ -4786,17 +4863,15 @@
         <v>39</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>91</v>
+        <v>232</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>39</v>
@@ -4845,69 +4920,65 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>39</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>191</v>
+        <v>39</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>39</v>
       </c>
@@ -4931,13 +5002,13 @@
         <v>39</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>39</v>
+        <v>240</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>39</v>
+        <v>241</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
@@ -4955,33 +5026,33 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>194</v>
+        <v>237</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>89</v>
+        <v>242</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>39</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5004,15 +5075,17 @@
         <v>39</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>246</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>247</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>39</v>
@@ -5037,13 +5110,13 @@
         <v>39</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>39</v>
+        <v>248</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>39</v>
+        <v>249</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>39</v>
@@ -5061,7 +5134,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5073,21 +5146,21 @@
         <v>39</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5107,19 +5180,23 @@
         <v>39</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>135</v>
+        <v>253</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>39</v>
       </c>
@@ -5143,13 +5220,13 @@
         <v>39</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>139</v>
+        <v>258</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>39</v>
@@ -5167,7 +5244,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5179,21 +5256,21 @@
         <v>39</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>39</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5216,13 +5293,13 @@
         <v>39</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>261</v>
+        <v>194</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5273,7 +5350,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5285,16 +5362,16 @@
         <v>39</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>265</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" hidden="true">
@@ -5322,13 +5399,13 @@
         <v>39</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>267</v>
+        <v>200</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>268</v>
+        <v>201</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5379,7 +5456,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5394,7 +5471,7 @@
         <v>39</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>39</v>
@@ -5405,11 +5482,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5428,15 +5505,17 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>270</v>
+        <v>205</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M40" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>39</v>
@@ -5485,7 +5564,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>269</v>
+        <v>207</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5497,10 +5576,10 @@
         <v>39</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>177</v>
+        <v>98</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>272</v>
+        <v>203</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>39</v>
@@ -5511,39 +5590,43 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>181</v>
+        <v>92</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>39</v>
       </c>
@@ -5591,22 +5674,22 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>39</v>
@@ -5617,18 +5700,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>39</v>
@@ -5640,17 +5723,15 @@
         <v>39</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>187</v>
+        <v>270</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>39</v>
@@ -5699,22 +5780,22 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>189</v>
+        <v>269</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>185</v>
+        <v>272</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>39</v>
@@ -5725,43 +5806,39 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>191</v>
+        <v>39</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>192</v>
+        <v>274</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>39</v>
       </c>
@@ -5785,13 +5862,13 @@
         <v>39</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>39</v>
+        <v>276</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>39</v>
+        <v>277</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>39</v>
@@ -5809,22 +5886,22 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>194</v>
+        <v>273</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>39</v>
@@ -5835,7 +5912,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5855,16 +5932,16 @@
         <v>39</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>113</v>
+        <v>279</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5915,7 +5992,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -5927,21 +6004,21 @@
         <v>39</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>116</v>
+        <v>282</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5964,13 +6041,13 @@
         <v>39</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6021,7 +6098,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6033,10 +6110,10 @@
         <v>39</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>283</v>
+        <v>224</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>39</v>
@@ -6047,7 +6124,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6058,7 +6135,7 @@
         <v>40</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>39</v>
@@ -6070,13 +6147,13 @@
         <v>39</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6103,57 +6180,57 @@
         <v>39</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="X46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE46" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="Y46" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="Z46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>284</v>
-      </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>142</v>
+        <v>290</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>289</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6176,13 +6253,13 @@
         <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>214</v>
+        <v>49</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>291</v>
+        <v>200</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>292</v>
+        <v>201</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6233,7 +6310,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>290</v>
+        <v>202</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6248,29 +6325,29 @@
         <v>39</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>293</v>
+        <v>203</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>294</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>39</v>
@@ -6282,15 +6359,17 @@
         <v>39</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>214</v>
+        <v>92</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>296</v>
+        <v>205</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="M48" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6339,65 +6418,69 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>295</v>
+        <v>207</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>298</v>
+        <v>203</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>299</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>301</v>
+        <v>92</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>302</v>
+        <v>210</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>39</v>
       </c>
@@ -6421,13 +6504,13 @@
         <v>39</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>304</v>
+        <v>39</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>305</v>
+        <v>39</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>39</v>
@@ -6445,33 +6528,33 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>300</v>
+        <v>212</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>306</v>
+        <v>90</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>307</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6494,20 +6577,16 @@
         <v>48</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>312</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>39</v>
       </c>
@@ -6531,13 +6610,13 @@
         <v>39</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>313</v>
+        <v>39</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>314</v>
+        <v>39</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>39</v>
@@ -6555,7 +6634,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6567,21 +6646,21 @@
         <v>39</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>315</v>
+        <v>297</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6592,10 +6671,10 @@
         <v>40</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>39</v>
@@ -6604,13 +6683,13 @@
         <v>39</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>317</v>
+        <v>49</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>12</v>
+        <v>299</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6661,32 +6740,672 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="AF51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG51" t="s" s="2">
+      <c r="AK54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F56" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AH51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>320</v>
+      <c r="G56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL51">
+  <autoFilter ref="A1:AL57">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6696,7 +7415,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI50">
+  <conditionalFormatting sqref="A2:AI56">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>